<commit_message>
se modif el excel
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor.xlsx
+++ b/Sura/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0719CED8-E40C-4C7D-AE85-25739BE2AEAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B652A1-265F-4631-9115-DA30B289DD93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1526,7 +1526,7 @@
   <dimension ref="A1:AC103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3:W103"/>
+      <selection activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se sube al master.
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor.xlsx
+++ b/Sura/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE21B70D-364D-4FCC-A3B8-2266F12C13DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0B1AAB-6212-4AFF-834D-470C415A8AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se modif excel para emitir polizas ara nacho
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor.xlsx
+++ b/Sura/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271D7FAF-C20D-4D12-A1C1-5A251D11EC14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89B7032-54F6-4E8F-A59E-C6BAD8CB9E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="376">
   <si>
     <t>Usuario</t>
   </si>
@@ -227,18 +227,6 @@
     <t>18/09/2020</t>
   </si>
   <si>
-    <t>RFA035</t>
-  </si>
-  <si>
-    <t>ABC12SRFA035</t>
-  </si>
-  <si>
-    <t>ZAZ123SRFA035</t>
-  </si>
-  <si>
-    <t>RFA036</t>
-  </si>
-  <si>
     <t>RFA037</t>
   </si>
   <si>
@@ -335,9 +323,6 @@
     <t>RFA068</t>
   </si>
   <si>
-    <t>ABC12SRFA036</t>
-  </si>
-  <si>
     <t>ABC12SRFA037</t>
   </si>
   <si>
@@ -434,9 +419,6 @@
     <t>ABC12SRFA068</t>
   </si>
   <si>
-    <t>ZAZ123SRFA036</t>
-  </si>
-  <si>
     <t>ZAZ123SRFA037</t>
   </si>
   <si>
@@ -1158,6 +1140,30 @@
   </si>
   <si>
     <t>6 meses</t>
+  </si>
+  <si>
+    <t>REN021</t>
+  </si>
+  <si>
+    <t>REN022</t>
+  </si>
+  <si>
+    <t>ABC12SREN021</t>
+  </si>
+  <si>
+    <t>ABC12SREN022</t>
+  </si>
+  <si>
+    <t>ZAZ123SREN021</t>
+  </si>
+  <si>
+    <t>ZAZ123SREN022</t>
+  </si>
+  <si>
+    <t>10/03/2020</t>
+  </si>
+  <si>
+    <t>Anual</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1231,6 +1237,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1539,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I102" sqref="I102:I103"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,8 +1684,8 @@
       <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="3">
-        <v>5712176326</v>
+      <c r="F2" s="10">
+        <v>2768688947</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -1685,10 +1694,10 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>375</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>46</v>
+        <v>374</v>
       </c>
       <c r="K2" t="s">
         <v>17</v>
@@ -1697,7 +1706,7 @@
         <v>41</v>
       </c>
       <c r="S2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="T2" t="s">
         <v>44</v>
@@ -1715,13 +1724,13 @@
         <v>40</v>
       </c>
       <c r="Y2" t="s">
-        <v>63</v>
+        <v>368</v>
       </c>
       <c r="Z2" t="s">
-        <v>64</v>
+        <v>370</v>
       </c>
       <c r="AA2" t="s">
-        <v>65</v>
+        <v>372</v>
       </c>
       <c r="AB2" t="s">
         <v>18</v>
@@ -1747,8 +1756,8 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="3">
-        <v>5712176326</v>
+      <c r="F3" s="10">
+        <v>2768688947</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
@@ -1757,10 +1766,10 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>375</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>46</v>
+        <v>374</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>
@@ -1769,7 +1778,7 @@
         <v>41</v>
       </c>
       <c r="S3">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="T3" t="s">
         <v>44</v>
@@ -1787,13 +1796,13 @@
         <v>40</v>
       </c>
       <c r="Y3" t="s">
-        <v>66</v>
+        <v>369</v>
       </c>
       <c r="Z3" t="s">
-        <v>99</v>
+        <v>371</v>
       </c>
       <c r="AA3" t="s">
-        <v>132</v>
+        <v>373</v>
       </c>
       <c r="AB3" t="s">
         <v>18</v>
@@ -1859,13 +1868,13 @@
         <v>40</v>
       </c>
       <c r="Y4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Z4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AA4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="AB4" t="s">
         <v>18</v>
@@ -1931,13 +1940,13 @@
         <v>40</v>
       </c>
       <c r="Y5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="Z5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="AA5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="AB5" t="s">
         <v>18</v>
@@ -2003,13 +2012,13 @@
         <v>40</v>
       </c>
       <c r="Y6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Z6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="AA6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="AB6" t="s">
         <v>18</v>
@@ -2075,13 +2084,13 @@
         <v>40</v>
       </c>
       <c r="Y7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="Z7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="AA7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="AB7" t="s">
         <v>18</v>
@@ -2117,13 +2126,13 @@
         <v>16</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>49</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>41</v>
@@ -2153,13 +2162,13 @@
         <v>40</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>18</v>
@@ -2195,13 +2204,13 @@
         <v>16</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>49</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>41</v>
@@ -2231,13 +2240,13 @@
         <v>40</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Z9" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AB9" s="5" t="s">
         <v>18</v>
@@ -2273,13 +2282,13 @@
         <v>16</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>50</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>41</v>
@@ -2309,13 +2318,13 @@
         <v>40</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="Z10" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>18</v>
@@ -2351,13 +2360,13 @@
         <v>16</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>50</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>41</v>
@@ -2387,13 +2396,13 @@
         <v>40</v>
       </c>
       <c r="Y11" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="Z11" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="AA11" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AB11" s="5" t="s">
         <v>18</v>
@@ -2429,13 +2438,13 @@
         <v>16</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>51</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>41</v>
@@ -2465,13 +2474,13 @@
         <v>40</v>
       </c>
       <c r="Y12" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Z12" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AA12" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="AB12" s="5" t="s">
         <v>18</v>
@@ -2507,13 +2516,13 @@
         <v>16</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>51</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>41</v>
@@ -2543,13 +2552,13 @@
         <v>40</v>
       </c>
       <c r="Y13" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="Z13" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="AB13" s="5" t="s">
         <v>18</v>
@@ -2585,13 +2594,13 @@
         <v>16</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>41</v>
@@ -2621,13 +2630,13 @@
         <v>40</v>
       </c>
       <c r="Y14" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AA14" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="AB14" s="5" t="s">
         <v>18</v>
@@ -2663,13 +2672,13 @@
         <v>16</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>41</v>
@@ -2699,13 +2708,13 @@
         <v>40</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Z15" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="AB15" s="5" t="s">
         <v>18</v>
@@ -2741,7 +2750,7 @@
         <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>53</v>
@@ -2771,13 +2780,13 @@
         <v>40</v>
       </c>
       <c r="Y16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Z16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AA16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AB16" t="s">
         <v>18</v>
@@ -2813,7 +2822,7 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>53</v>
@@ -2843,13 +2852,13 @@
         <v>40</v>
       </c>
       <c r="Y17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="Z17" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="AA17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="AB17" t="s">
         <v>18</v>
@@ -2885,7 +2894,7 @@
         <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>54</v>
@@ -2915,13 +2924,13 @@
         <v>40</v>
       </c>
       <c r="Y18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Z18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="AA18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AB18" t="s">
         <v>18</v>
@@ -2957,7 +2966,7 @@
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>54</v>
@@ -2987,13 +2996,13 @@
         <v>40</v>
       </c>
       <c r="Y19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Z19" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="AA19" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="AB19" t="s">
         <v>18</v>
@@ -3029,7 +3038,7 @@
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>55</v>
@@ -3059,13 +3068,13 @@
         <v>40</v>
       </c>
       <c r="Y20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="Z20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AA20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="AB20" t="s">
         <v>18</v>
@@ -3101,7 +3110,7 @@
         <v>16</v>
       </c>
       <c r="I21" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>55</v>
@@ -3131,13 +3140,13 @@
         <v>40</v>
       </c>
       <c r="Y21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="Z21" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AA21" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="AB21" t="s">
         <v>18</v>
@@ -3173,7 +3182,7 @@
         <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>56</v>
@@ -3212,13 +3221,13 @@
         <v>40</v>
       </c>
       <c r="Y22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="Z22" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AA22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AB22" t="s">
         <v>18</v>
@@ -3254,7 +3263,7 @@
         <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>56</v>
@@ -3290,13 +3299,13 @@
         <v>40</v>
       </c>
       <c r="Y23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="Z23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="AA23" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="AB23" t="s">
         <v>18</v>
@@ -3332,7 +3341,7 @@
         <v>16</v>
       </c>
       <c r="I24" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>57</v>
@@ -3368,13 +3377,13 @@
         <v>40</v>
       </c>
       <c r="Y24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="Z24" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="AA24" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="AB24" t="s">
         <v>18</v>
@@ -3410,7 +3419,7 @@
         <v>16</v>
       </c>
       <c r="I25" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>57</v>
@@ -3440,13 +3449,13 @@
         <v>40</v>
       </c>
       <c r="Y25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="Z25" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="AA25" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AB25" t="s">
         <v>18</v>
@@ -3482,7 +3491,7 @@
         <v>16</v>
       </c>
       <c r="I26" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>58</v>
@@ -3514,13 +3523,13 @@
         <v>40</v>
       </c>
       <c r="Y26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Z26" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AA26" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="AB26" t="s">
         <v>18</v>
@@ -3556,7 +3565,7 @@
         <v>16</v>
       </c>
       <c r="I27" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>58</v>
@@ -3587,13 +3596,13 @@
         <v>40</v>
       </c>
       <c r="Y27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Z27" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AA27" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="AB27" t="s">
         <v>18</v>
@@ -3629,13 +3638,13 @@
         <v>16</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>41</v>
@@ -3665,13 +3674,13 @@
         <v>40</v>
       </c>
       <c r="Y28" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Z28" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="AA28" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="AB28" s="5" t="s">
         <v>18</v>
@@ -3707,13 +3716,13 @@
         <v>16</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>41</v>
@@ -3743,13 +3752,13 @@
         <v>40</v>
       </c>
       <c r="Y29" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Z29" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AA29" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AB29" s="5" t="s">
         <v>18</v>
@@ -3815,13 +3824,13 @@
         <v>40</v>
       </c>
       <c r="Y30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Z30" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="AA30" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="AB30" t="s">
         <v>18</v>
@@ -3887,13 +3896,13 @@
         <v>40</v>
       </c>
       <c r="Y31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="Z31" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="AA31" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="AB31" t="s">
         <v>18</v>
@@ -3929,7 +3938,7 @@
         <v>16</v>
       </c>
       <c r="I32" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>61</v>
@@ -3959,13 +3968,13 @@
         <v>40</v>
       </c>
       <c r="Y32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Z32" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AA32" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="AB32" t="s">
         <v>18</v>
@@ -4001,7 +4010,7 @@
         <v>16</v>
       </c>
       <c r="I33" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>61</v>
@@ -4031,13 +4040,13 @@
         <v>40</v>
       </c>
       <c r="Y33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Z33" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="AA33" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="AB33" t="s">
         <v>18</v>
@@ -4073,7 +4082,7 @@
         <v>16</v>
       </c>
       <c r="I34" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>62</v>
@@ -4103,13 +4112,13 @@
         <v>40</v>
       </c>
       <c r="Y34" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Z34" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="AA34" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="AB34" t="s">
         <v>18</v>
@@ -4145,7 +4154,7 @@
         <v>16</v>
       </c>
       <c r="I35" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>62</v>
@@ -4175,13 +4184,13 @@
         <v>40</v>
       </c>
       <c r="Y35" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="Z35" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AA35" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="AB35" t="s">
         <v>18</v>
@@ -4247,13 +4256,13 @@
         <v>40</v>
       </c>
       <c r="Y36" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="Z36" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AA36" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AB36" t="s">
         <v>18</v>
@@ -4319,13 +4328,13 @@
         <v>40</v>
       </c>
       <c r="Y37" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="Z37" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="AA37" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AB37" t="s">
         <v>18</v>
@@ -4391,13 +4400,13 @@
         <v>40</v>
       </c>
       <c r="Y38" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="Z38" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AA38" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="AB38" t="s">
         <v>18</v>
@@ -4463,13 +4472,13 @@
         <v>40</v>
       </c>
       <c r="Y39" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="Z39" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="AA39" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="AB39" t="s">
         <v>18</v>
@@ -4535,13 +4544,13 @@
         <v>40</v>
       </c>
       <c r="Y40" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="Z40" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="AA40" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="AB40" t="s">
         <v>18</v>
@@ -4607,13 +4616,13 @@
         <v>40</v>
       </c>
       <c r="Y41" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Z41" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="AA41" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="AB41" t="s">
         <v>18</v>
@@ -4649,13 +4658,13 @@
         <v>16</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>49</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>41</v>
@@ -4685,13 +4694,13 @@
         <v>40</v>
       </c>
       <c r="Y42" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="Z42" s="5" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="AA42" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="AB42" s="5" t="s">
         <v>18</v>
@@ -4727,13 +4736,13 @@
         <v>16</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>49</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>41</v>
@@ -4763,13 +4772,13 @@
         <v>40</v>
       </c>
       <c r="Y43" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="Z43" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="AA43" s="5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="AB43" s="5" t="s">
         <v>18</v>
@@ -4805,13 +4814,13 @@
         <v>16</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>50</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>41</v>
@@ -4841,13 +4850,13 @@
         <v>40</v>
       </c>
       <c r="Y44" s="5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="Z44" s="5" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="AA44" s="5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="AB44" s="5" t="s">
         <v>18</v>
@@ -4883,13 +4892,13 @@
         <v>16</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J45" s="8" t="s">
         <v>50</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>41</v>
@@ -4919,13 +4928,13 @@
         <v>40</v>
       </c>
       <c r="Y45" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="Z45" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="AA45" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AB45" s="5" t="s">
         <v>18</v>
@@ -4961,13 +4970,13 @@
         <v>16</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J46" s="8" t="s">
         <v>51</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>41</v>
@@ -4997,13 +5006,13 @@
         <v>40</v>
       </c>
       <c r="Y46" s="5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="Z46" s="5" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="AA46" s="5" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="AB46" s="5" t="s">
         <v>18</v>
@@ -5039,13 +5048,13 @@
         <v>16</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>51</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>41</v>
@@ -5075,13 +5084,13 @@
         <v>40</v>
       </c>
       <c r="Y47" s="5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="Z47" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="AA47" s="5" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="AB47" s="5" t="s">
         <v>18</v>
@@ -5117,13 +5126,13 @@
         <v>16</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J48" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>41</v>
@@ -5153,13 +5162,13 @@
         <v>40</v>
       </c>
       <c r="Y48" s="5" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="Z48" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="AA48" s="5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="AB48" s="5" t="s">
         <v>18</v>
@@ -5195,13 +5204,13 @@
         <v>16</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J49" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>41</v>
@@ -5231,13 +5240,13 @@
         <v>40</v>
       </c>
       <c r="Y49" s="5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="Z49" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="AA49" s="5" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="AB49" s="5" t="s">
         <v>18</v>
@@ -5273,7 +5282,7 @@
         <v>16</v>
       </c>
       <c r="I50" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>53</v>
@@ -5303,13 +5312,13 @@
         <v>40</v>
       </c>
       <c r="Y50" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="Z50" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="AA50" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="AB50" t="s">
         <v>18</v>
@@ -5345,7 +5354,7 @@
         <v>16</v>
       </c>
       <c r="I51" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>53</v>
@@ -5375,13 +5384,13 @@
         <v>40</v>
       </c>
       <c r="Y51" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="Z51" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="AA51" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="AB51" t="s">
         <v>18</v>
@@ -5417,7 +5426,7 @@
         <v>16</v>
       </c>
       <c r="I52" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>54</v>
@@ -5447,13 +5456,13 @@
         <v>40</v>
       </c>
       <c r="Y52" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="Z52" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AA52" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="AB52" t="s">
         <v>18</v>
@@ -5489,7 +5498,7 @@
         <v>16</v>
       </c>
       <c r="I53" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>54</v>
@@ -5519,13 +5528,13 @@
         <v>40</v>
       </c>
       <c r="Y53" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="Z53" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="AA53" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="AB53" t="s">
         <v>18</v>
@@ -5561,7 +5570,7 @@
         <v>16</v>
       </c>
       <c r="I54" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>55</v>
@@ -5591,13 +5600,13 @@
         <v>40</v>
       </c>
       <c r="Y54" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="Z54" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="AA54" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="AB54" t="s">
         <v>18</v>
@@ -5633,7 +5642,7 @@
         <v>16</v>
       </c>
       <c r="I55" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>55</v>
@@ -5663,13 +5672,13 @@
         <v>40</v>
       </c>
       <c r="Y55" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="Z55" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA55" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="AB55" t="s">
         <v>18</v>
@@ -5705,7 +5714,7 @@
         <v>16</v>
       </c>
       <c r="I56" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>56</v>
@@ -5735,13 +5744,13 @@
         <v>40</v>
       </c>
       <c r="Y56" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="Z56" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="AA56" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="AB56" t="s">
         <v>18</v>
@@ -5777,7 +5786,7 @@
         <v>16</v>
       </c>
       <c r="I57" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>56</v>
@@ -5807,13 +5816,13 @@
         <v>40</v>
       </c>
       <c r="Y57" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="Z57" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="AA57" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="AB57" t="s">
         <v>18</v>
@@ -5849,7 +5858,7 @@
         <v>16</v>
       </c>
       <c r="I58" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>57</v>
@@ -5879,13 +5888,13 @@
         <v>40</v>
       </c>
       <c r="Y58" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="Z58" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="AA58" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="AB58" t="s">
         <v>18</v>
@@ -5921,7 +5930,7 @@
         <v>16</v>
       </c>
       <c r="I59" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>57</v>
@@ -5951,13 +5960,13 @@
         <v>40</v>
       </c>
       <c r="Y59" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="Z59" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="AA59" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="AB59" t="s">
         <v>18</v>
@@ -5993,7 +6002,7 @@
         <v>16</v>
       </c>
       <c r="I60" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>58</v>
@@ -6023,13 +6032,13 @@
         <v>40</v>
       </c>
       <c r="Y60" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="Z60" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="AA60" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="AB60" t="s">
         <v>18</v>
@@ -6065,7 +6074,7 @@
         <v>16</v>
       </c>
       <c r="I61" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>58</v>
@@ -6095,13 +6104,13 @@
         <v>40</v>
       </c>
       <c r="Y61" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="Z61" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="AA61" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="AB61" t="s">
         <v>18</v>
@@ -6137,13 +6146,13 @@
         <v>16</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J62" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L62" s="5" t="s">
         <v>41</v>
@@ -6173,13 +6182,13 @@
         <v>40</v>
       </c>
       <c r="Y62" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="Z62" s="5" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="AA62" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AB62" s="5" t="s">
         <v>18</v>
@@ -6215,13 +6224,13 @@
         <v>16</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J63" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L63" s="5" t="s">
         <v>41</v>
@@ -6251,13 +6260,13 @@
         <v>40</v>
       </c>
       <c r="Y63" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="Z63" s="5" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AA63" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AB63" s="5" t="s">
         <v>18</v>
@@ -6323,13 +6332,13 @@
         <v>40</v>
       </c>
       <c r="Y64" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="Z64" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="AA64" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="AB64" t="s">
         <v>18</v>
@@ -6395,13 +6404,13 @@
         <v>40</v>
       </c>
       <c r="Y65" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="Z65" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="AA65" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="AB65" t="s">
         <v>18</v>
@@ -6437,7 +6446,7 @@
         <v>16</v>
       </c>
       <c r="I66" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>61</v>
@@ -6467,13 +6476,13 @@
         <v>40</v>
       </c>
       <c r="Y66" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="Z66" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AA66" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="AB66" t="s">
         <v>18</v>
@@ -6509,7 +6518,7 @@
         <v>16</v>
       </c>
       <c r="I67" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>61</v>
@@ -6539,13 +6548,13 @@
         <v>40</v>
       </c>
       <c r="Y67" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="Z67" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="AA67" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="AB67" t="s">
         <v>18</v>
@@ -6581,7 +6590,7 @@
         <v>16</v>
       </c>
       <c r="I68" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>62</v>
@@ -6611,13 +6620,13 @@
         <v>40</v>
       </c>
       <c r="Y68" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="Z68" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="AA68" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="AB68" t="s">
         <v>18</v>
@@ -6653,7 +6662,7 @@
         <v>16</v>
       </c>
       <c r="I69" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>62</v>
@@ -6683,13 +6692,13 @@
         <v>40</v>
       </c>
       <c r="Y69" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="Z69" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AA69" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="AB69" t="s">
         <v>18</v>
@@ -6755,13 +6764,13 @@
         <v>40</v>
       </c>
       <c r="Y70" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="Z70" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="AA70" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AB70" t="s">
         <v>18</v>
@@ -6827,13 +6836,13 @@
         <v>40</v>
       </c>
       <c r="Y71" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="Z71" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="AA71" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="AB71" t="s">
         <v>18</v>
@@ -6899,13 +6908,13 @@
         <v>40</v>
       </c>
       <c r="Y72" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="Z72" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="AA72" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="AB72" t="s">
         <v>18</v>
@@ -6971,13 +6980,13 @@
         <v>40</v>
       </c>
       <c r="Y73" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="Z73" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="AA73" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="AB73" t="s">
         <v>18</v>
@@ -7043,13 +7052,13 @@
         <v>40</v>
       </c>
       <c r="Y74" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="Z74" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="AA74" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="AB74" t="s">
         <v>18</v>
@@ -7115,13 +7124,13 @@
         <v>40</v>
       </c>
       <c r="Y75" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="Z75" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="AA75" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="AB75" t="s">
         <v>18</v>
@@ -7157,13 +7166,13 @@
         <v>16</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J76" s="8" t="s">
         <v>49</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L76" s="5" t="s">
         <v>41</v>
@@ -7193,13 +7202,13 @@
         <v>40</v>
       </c>
       <c r="Y76" s="5" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="Z76" s="5" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="AA76" s="5" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="AB76" s="5" t="s">
         <v>18</v>
@@ -7235,13 +7244,13 @@
         <v>16</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J77" s="8" t="s">
         <v>49</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L77" s="5" t="s">
         <v>41</v>
@@ -7271,13 +7280,13 @@
         <v>40</v>
       </c>
       <c r="Y77" s="5" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Z77" s="5" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="AA77" s="5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="AB77" s="5" t="s">
         <v>18</v>
@@ -7313,13 +7322,13 @@
         <v>16</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J78" s="8" t="s">
         <v>50</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L78" s="5" t="s">
         <v>41</v>
@@ -7349,13 +7358,13 @@
         <v>40</v>
       </c>
       <c r="Y78" s="5" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="Z78" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="AA78" s="5" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="AB78" s="5" t="s">
         <v>18</v>
@@ -7391,13 +7400,13 @@
         <v>16</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J79" s="8" t="s">
         <v>50</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L79" s="5" t="s">
         <v>41</v>
@@ -7427,13 +7436,13 @@
         <v>40</v>
       </c>
       <c r="Y79" s="5" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="Z79" s="5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="AA79" s="5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="AB79" s="5" t="s">
         <v>18</v>
@@ -7469,13 +7478,13 @@
         <v>16</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J80" s="8" t="s">
         <v>51</v>
       </c>
       <c r="K80" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L80" s="5" t="s">
         <v>41</v>
@@ -7505,13 +7514,13 @@
         <v>40</v>
       </c>
       <c r="Y80" s="5" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="Z80" s="5" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="AA80" s="5" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="AB80" s="5" t="s">
         <v>18</v>
@@ -7547,13 +7556,13 @@
         <v>16</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J81" s="8" t="s">
         <v>51</v>
       </c>
       <c r="K81" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L81" s="5" t="s">
         <v>41</v>
@@ -7583,13 +7592,13 @@
         <v>40</v>
       </c>
       <c r="Y81" s="5" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="Z81" s="5" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="AA81" s="5" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="AB81" s="5" t="s">
         <v>18</v>
@@ -7625,13 +7634,13 @@
         <v>16</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J82" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K82" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L82" s="5" t="s">
         <v>41</v>
@@ -7661,13 +7670,13 @@
         <v>40</v>
       </c>
       <c r="Y82" s="5" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="Z82" s="5" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="AA82" s="5" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="AB82" s="5" t="s">
         <v>18</v>
@@ -7703,13 +7712,13 @@
         <v>16</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J83" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K83" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L83" s="5" t="s">
         <v>41</v>
@@ -7739,13 +7748,13 @@
         <v>40</v>
       </c>
       <c r="Y83" s="5" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="Z83" s="5" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="AA83" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="AB83" s="5" t="s">
         <v>18</v>
@@ -7781,7 +7790,7 @@
         <v>16</v>
       </c>
       <c r="I84" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>53</v>
@@ -7811,13 +7820,13 @@
         <v>40</v>
       </c>
       <c r="Y84" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="Z84" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="AA84" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="AB84" t="s">
         <v>18</v>
@@ -7853,7 +7862,7 @@
         <v>16</v>
       </c>
       <c r="I85" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J85" s="4" t="s">
         <v>53</v>
@@ -7883,13 +7892,13 @@
         <v>40</v>
       </c>
       <c r="Y85" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="Z85" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="AA85" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AB85" t="s">
         <v>18</v>
@@ -7925,7 +7934,7 @@
         <v>16</v>
       </c>
       <c r="I86" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J86" s="4" t="s">
         <v>54</v>
@@ -7955,13 +7964,13 @@
         <v>40</v>
       </c>
       <c r="Y86" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="Z86" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="AA86" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="AB86" t="s">
         <v>18</v>
@@ -7997,7 +8006,7 @@
         <v>16</v>
       </c>
       <c r="I87" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>54</v>
@@ -8027,13 +8036,13 @@
         <v>40</v>
       </c>
       <c r="Y87" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="Z87" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="AA87" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="AB87" t="s">
         <v>18</v>
@@ -8069,7 +8078,7 @@
         <v>16</v>
       </c>
       <c r="I88" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>55</v>
@@ -8099,13 +8108,13 @@
         <v>40</v>
       </c>
       <c r="Y88" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="Z88" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="AA88" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="AB88" t="s">
         <v>18</v>
@@ -8141,7 +8150,7 @@
         <v>16</v>
       </c>
       <c r="I89" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>55</v>
@@ -8171,13 +8180,13 @@
         <v>40</v>
       </c>
       <c r="Y89" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="Z89" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="AA89" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="AB89" t="s">
         <v>18</v>
@@ -8213,7 +8222,7 @@
         <v>16</v>
       </c>
       <c r="I90" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J90" s="4" t="s">
         <v>56</v>
@@ -8243,13 +8252,13 @@
         <v>40</v>
       </c>
       <c r="Y90" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="Z90" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="AA90" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="AB90" t="s">
         <v>18</v>
@@ -8285,7 +8294,7 @@
         <v>16</v>
       </c>
       <c r="I91" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J91" s="4" t="s">
         <v>56</v>
@@ -8315,13 +8324,13 @@
         <v>40</v>
       </c>
       <c r="Y91" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="Z91" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="AA91" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="AB91" t="s">
         <v>18</v>
@@ -8357,7 +8366,7 @@
         <v>16</v>
       </c>
       <c r="I92" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J92" s="4" t="s">
         <v>57</v>
@@ -8387,13 +8396,13 @@
         <v>40</v>
       </c>
       <c r="Y92" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="Z92" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="AA92" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="AB92" t="s">
         <v>18</v>
@@ -8429,7 +8438,7 @@
         <v>16</v>
       </c>
       <c r="I93" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J93" s="4" t="s">
         <v>57</v>
@@ -8459,13 +8468,13 @@
         <v>40</v>
       </c>
       <c r="Y93" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="Z93" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="AA93" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="AB93" t="s">
         <v>18</v>
@@ -8501,7 +8510,7 @@
         <v>16</v>
       </c>
       <c r="I94" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J94" s="4" t="s">
         <v>58</v>
@@ -8531,13 +8540,13 @@
         <v>40</v>
       </c>
       <c r="Y94" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="Z94" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="AA94" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="AB94" t="s">
         <v>18</v>
@@ -8573,7 +8582,7 @@
         <v>16</v>
       </c>
       <c r="I95" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J95" s="4" t="s">
         <v>58</v>
@@ -8603,13 +8612,13 @@
         <v>40</v>
       </c>
       <c r="Y95" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="Z95" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="AA95" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AB95" t="s">
         <v>18</v>
@@ -8645,13 +8654,13 @@
         <v>16</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J96" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L96" s="5" t="s">
         <v>41</v>
@@ -8681,13 +8690,13 @@
         <v>40</v>
       </c>
       <c r="Y96" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="Z96" s="5" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AA96" s="5" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="AB96" s="5" t="s">
         <v>18</v>
@@ -8723,13 +8732,13 @@
         <v>16</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J97" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K97" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="L97" s="5" t="s">
         <v>41</v>
@@ -8759,13 +8768,13 @@
         <v>40</v>
       </c>
       <c r="Y97" s="5" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="Z97" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="AA97" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="AB97" s="5" t="s">
         <v>18</v>
@@ -8831,13 +8840,13 @@
         <v>40</v>
       </c>
       <c r="Y98" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="Z98" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="AA98" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="AB98" t="s">
         <v>18</v>
@@ -8903,13 +8912,13 @@
         <v>40</v>
       </c>
       <c r="Y99" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="Z99" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="AA99" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="AB99" t="s">
         <v>18</v>
@@ -8945,7 +8954,7 @@
         <v>16</v>
       </c>
       <c r="I100" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J100" s="4" t="s">
         <v>61</v>
@@ -8975,13 +8984,13 @@
         <v>40</v>
       </c>
       <c r="Y100" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="Z100" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="AA100" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="AB100" t="s">
         <v>18</v>
@@ -9017,7 +9026,7 @@
         <v>16</v>
       </c>
       <c r="I101" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J101" s="4" t="s">
         <v>61</v>
@@ -9047,13 +9056,13 @@
         <v>40</v>
       </c>
       <c r="Y101" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="Z101" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="AA101" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="AB101" t="s">
         <v>18</v>
@@ -9089,7 +9098,7 @@
         <v>16</v>
       </c>
       <c r="I102" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J102" s="4" t="s">
         <v>62</v>
@@ -9119,13 +9128,13 @@
         <v>40</v>
       </c>
       <c r="Y102" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="Z102" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="AA102" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="AB102" t="s">
         <v>18</v>
@@ -9161,7 +9170,7 @@
         <v>16</v>
       </c>
       <c r="I103" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J103" s="4" t="s">
         <v>62</v>
@@ -9191,13 +9200,13 @@
         <v>40</v>
       </c>
       <c r="Y103" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Z103" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="AA103" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="AB103" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
se sube ultima version para creación de tarea en jenkins EmisionMotorAist0km
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor.xlsx
+++ b/Sura/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89B7032-54F6-4E8F-A59E-C6BAD8CB9E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55272AB9-4D62-4690-AE33-8FDEC84B6394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,28 +1142,28 @@
     <t>6 meses</t>
   </si>
   <si>
-    <t>REN021</t>
-  </si>
-  <si>
-    <t>REN022</t>
-  </si>
-  <si>
-    <t>ABC12SREN021</t>
-  </si>
-  <si>
-    <t>ABC12SREN022</t>
-  </si>
-  <si>
-    <t>ZAZ123SREN021</t>
-  </si>
-  <si>
-    <t>ZAZ123SREN022</t>
-  </si>
-  <si>
-    <t>10/03/2020</t>
-  </si>
-  <si>
     <t>Anual</t>
+  </si>
+  <si>
+    <t>05/03/2020</t>
+  </si>
+  <si>
+    <t>REN023</t>
+  </si>
+  <si>
+    <t>ABC12SREN023</t>
+  </si>
+  <si>
+    <t>ZAZ123SREN023</t>
+  </si>
+  <si>
+    <t>REN024</t>
+  </si>
+  <si>
+    <t>ABC12SREN024</t>
+  </si>
+  <si>
+    <t>ZAZ123SREN024</t>
   </si>
 </sst>
 </file>
@@ -1549,7 +1549,7 @@
   <dimension ref="A1:AC103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="AA2" sqref="AA2:AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,10 +1694,10 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="K2" t="s">
         <v>17</v>
@@ -1724,10 +1724,10 @@
         <v>40</v>
       </c>
       <c r="Y2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="Z2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AA2" t="s">
         <v>372</v>
@@ -1766,10 +1766,10 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>
@@ -1796,13 +1796,13 @@
         <v>40</v>
       </c>
       <c r="Y3" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="Z3" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="AA3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="AB3" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
se modif datasources y se arregla item de Campaña y
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor.xlsx
+++ b/Sura/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A54BDF2-18A2-416C-91D9-3A0EB4820825}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CC0C18-0F06-436E-A176-BC1C6FADEC70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="82">
   <si>
     <t>Usuario</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Sin Actividad</t>
   </si>
   <si>
-    <t>su</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -158,18 +155,6 @@
     <t>preproducciongestion.segurossura.com.ar</t>
   </si>
   <si>
-    <t>silverarrow</t>
-  </si>
-  <si>
-    <t>10/03/2021</t>
-  </si>
-  <si>
-    <t>Tarjeta de Crédito</t>
-  </si>
-  <si>
-    <t>Débito Bancario</t>
-  </si>
-  <si>
     <t>Naranja</t>
   </si>
   <si>
@@ -185,31 +170,115 @@
     <t>0340010400044915199004</t>
   </si>
   <si>
-    <t>RPM001</t>
-  </si>
-  <si>
-    <t>ABC12SRPM001</t>
-  </si>
-  <si>
-    <t>ZAZ123SRPM001</t>
-  </si>
-  <si>
-    <t>RPM002</t>
-  </si>
-  <si>
-    <t>RPM003</t>
-  </si>
-  <si>
-    <t>ABC12SRPM002</t>
-  </si>
-  <si>
-    <t>ABC12SRPM003</t>
-  </si>
-  <si>
-    <t>ZAZ123SRPM002</t>
-  </si>
-  <si>
-    <t>ZAZ123SRPM003</t>
+    <t>garcianico</t>
+  </si>
+  <si>
+    <t>gw</t>
+  </si>
+  <si>
+    <t>22/03/2021</t>
+  </si>
+  <si>
+    <t>PRP001</t>
+  </si>
+  <si>
+    <t>PRP002</t>
+  </si>
+  <si>
+    <t>PRP003</t>
+  </si>
+  <si>
+    <t>ABC12SPRP001</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP001</t>
+  </si>
+  <si>
+    <t>ABC12SPRP002</t>
+  </si>
+  <si>
+    <t>ABC12SPRP003</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP002</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP003</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>RENAULT</t>
+  </si>
+  <si>
+    <t>LOGAN II 1.6 8V EXPRESSION</t>
+  </si>
+  <si>
+    <t>B - Resp. Civil-Robo/Incendio Total Daños Totales por Accidente</t>
+  </si>
+  <si>
+    <t>PRP004</t>
+  </si>
+  <si>
+    <t>PRP005</t>
+  </si>
+  <si>
+    <t>PRP006</t>
+  </si>
+  <si>
+    <t>PRP007</t>
+  </si>
+  <si>
+    <t>PRP008</t>
+  </si>
+  <si>
+    <t>PRP009</t>
+  </si>
+  <si>
+    <t>PRP010</t>
+  </si>
+  <si>
+    <t>ABC12SPRP004</t>
+  </si>
+  <si>
+    <t>ABC12SPRP005</t>
+  </si>
+  <si>
+    <t>ABC12SPRP006</t>
+  </si>
+  <si>
+    <t>ABC12SPRP007</t>
+  </si>
+  <si>
+    <t>ABC12SPRP008</t>
+  </si>
+  <si>
+    <t>ABC12SPRP009</t>
+  </si>
+  <si>
+    <t>ABC12SPRP010</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP004</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP005</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP006</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP007</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP008</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP009</t>
+  </si>
+  <si>
+    <t>ZAZ123SPRP010</t>
   </si>
 </sst>
 </file>
@@ -553,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6:AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +633,7 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.28515625" customWidth="1"/>
     <col min="3" max="3" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
@@ -587,13 +656,13 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -611,10 +680,10 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
         <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
@@ -623,28 +692,28 @@
         <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
-      </c>
-      <c r="R1" t="s">
-        <v>29</v>
       </c>
       <c r="S1" t="s">
         <v>7</v>
       </c>
       <c r="T1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U1" t="s">
         <v>8</v>
@@ -671,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="AC1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -679,19 +748,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F2" s="4">
-        <v>2617100594</v>
+        <v>1865378806</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -700,37 +769,37 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="K2" t="s">
         <v>17</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S2">
         <v>2021</v>
       </c>
       <c r="T2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" t="s">
         <v>30</v>
-      </c>
-      <c r="V2" t="s">
-        <v>31</v>
       </c>
       <c r="W2">
         <v>1380000</v>
       </c>
       <c r="X2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Z2" t="s">
         <v>51</v>
@@ -742,7 +811,7 @@
         <v>18</v>
       </c>
       <c r="AC2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -750,19 +819,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F3" s="4">
-        <v>2617100594</v>
+        <v>1865378806</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
@@ -771,58 +840,58 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="K3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="S3">
         <v>2021</v>
       </c>
       <c r="T3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" t="s">
         <v>30</v>
-      </c>
-      <c r="V3" t="s">
-        <v>31</v>
       </c>
       <c r="W3">
         <v>1380000</v>
       </c>
       <c r="X3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" t="s">
         <v>53</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>55</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>57</v>
       </c>
       <c r="AB3" t="s">
         <v>18</v>
       </c>
       <c r="AC3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -830,19 +899,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F4" s="4">
-        <v>2617100594</v>
+        <v>1865378806</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -851,55 +920,564 @@
         <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>48</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="S4">
         <v>2021</v>
       </c>
       <c r="T4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" t="s">
         <v>30</v>
-      </c>
-      <c r="V4" t="s">
-        <v>31</v>
       </c>
       <c r="W4">
         <v>1380000</v>
       </c>
       <c r="X4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z4" t="s">
         <v>54</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>56</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>58</v>
       </c>
       <c r="AB4" t="s">
         <v>18</v>
       </c>
       <c r="AC4" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1865378806</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5">
+        <v>2021</v>
+      </c>
+      <c r="T5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" t="s">
+        <v>30</v>
+      </c>
+      <c r="W5">
+        <v>1380000</v>
+      </c>
+      <c r="X5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1865378806</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6">
+        <v>2021</v>
+      </c>
+      <c r="T6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" t="s">
+        <v>29</v>
+      </c>
+      <c r="V6" t="s">
+        <v>30</v>
+      </c>
+      <c r="W6">
+        <v>1380000</v>
+      </c>
+      <c r="X6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="4">
+        <v>6404770682</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7">
+        <v>2018</v>
+      </c>
+      <c r="T7" t="s">
+        <v>57</v>
+      </c>
+      <c r="U7" t="s">
+        <v>58</v>
+      </c>
+      <c r="V7" t="s">
+        <v>59</v>
+      </c>
+      <c r="W7">
+        <v>1200000</v>
+      </c>
+      <c r="X7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="4">
+        <v>6404770682</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S8">
+        <v>2018</v>
+      </c>
+      <c r="T8" t="s">
+        <v>57</v>
+      </c>
+      <c r="U8" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" t="s">
+        <v>59</v>
+      </c>
+      <c r="W8">
+        <v>1200000</v>
+      </c>
+      <c r="X8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="4">
+        <v>6404770682</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9">
+        <v>2018</v>
+      </c>
+      <c r="T9" t="s">
+        <v>57</v>
+      </c>
+      <c r="U9" t="s">
+        <v>58</v>
+      </c>
+      <c r="V9" t="s">
+        <v>59</v>
+      </c>
+      <c r="W9">
+        <v>1200000</v>
+      </c>
+      <c r="X9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="4">
+        <v>6404770682</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10">
+        <v>2018</v>
+      </c>
+      <c r="T10" t="s">
+        <v>57</v>
+      </c>
+      <c r="U10" t="s">
+        <v>58</v>
+      </c>
+      <c r="V10" t="s">
+        <v>59</v>
+      </c>
+      <c r="W10">
+        <v>1200000</v>
+      </c>
+      <c r="X10" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4">
+        <v>6404770682</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11">
+        <v>2018</v>
+      </c>
+      <c r="T11" t="s">
+        <v>57</v>
+      </c>
+      <c r="U11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V11" t="s">
+        <v>59</v>
+      </c>
+      <c r="W11">
+        <v>1200000</v>
+      </c>
+      <c r="X11" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se sube item campaña arreglado de nuevo
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor.xlsx
+++ b/Sura/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CC0C18-0F06-436E-A176-BC1C6FADEC70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB971E73-0A1D-41A9-ABA9-62C824CB6563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,6 +155,9 @@
     <t>preproducciongestion.segurossura.com.ar</t>
   </si>
   <si>
+    <t>silverarrow</t>
+  </si>
+  <si>
     <t>Naranja</t>
   </si>
   <si>
@@ -171,9 +174,6 @@
   </si>
   <si>
     <t>garcianico</t>
-  </si>
-  <si>
-    <t>gw</t>
   </si>
   <si>
     <t>22/03/2021</t>
@@ -625,7 +625,7 @@
   <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6:AC11"/>
+      <selection activeCell="E3" sqref="E3:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,10 +754,10 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F2" s="4">
         <v>1865378806</v>
@@ -825,10 +825,10 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F3" s="4">
         <v>1865378806</v>
@@ -852,13 +852,13 @@
         <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S3">
         <v>2021</v>
@@ -905,10 +905,10 @@
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F4" s="4">
         <v>1865378806</v>
@@ -932,10 +932,10 @@
         <v>33</v>
       </c>
       <c r="Q4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S4">
         <v>2021</v>
@@ -982,10 +982,10 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F5" s="4">
         <v>1865378806</v>
@@ -1009,10 +1009,10 @@
         <v>33</v>
       </c>
       <c r="Q5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S5">
         <v>2021</v>
@@ -1059,10 +1059,10 @@
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F6" s="4">
         <v>1865378806</v>
@@ -1086,10 +1086,10 @@
         <v>33</v>
       </c>
       <c r="Q6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S6">
         <v>2021</v>
@@ -1136,10 +1136,10 @@
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F7" s="4">
         <v>6404770682</v>
@@ -1207,10 +1207,10 @@
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F8" s="4">
         <v>6404770682</v>
@@ -1278,10 +1278,10 @@
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F9" s="4">
         <v>6404770682</v>
@@ -1349,10 +1349,10 @@
         <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F10" s="4">
         <v>6404770682</v>
@@ -1420,10 +1420,10 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F11" s="4">
         <v>6404770682</v>

</xml_diff>